<commit_message>
Create a link beteen main.py and read.py.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guestpub\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guestpub\Desktop\Programming\GitHub\MiniProject-CollectChineseBooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -37,9 +37,6 @@
     <t>Author</t>
   </si>
   <si>
-    <t>J. K. Rowling</t>
-  </si>
-  <si>
     <t>Publisher</t>
   </si>
   <si>
@@ -47,66 +44,32 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Harry Potter and the Sorcerer's Stone</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Harry Potter and the Chamber of Secrets</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Harry Potter and the Prisoner of Azkaban</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Harry Potter and the Goblet of Fire</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Harry Potter and the Order of the Phoenix</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Harry Potter and the Half-Blood Prince</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Harry Potter and the Deathly Hallows</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ISBN</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Scholastic </t>
-  </si>
-  <si>
-    <t>A Game of Thrones</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Clash of Kings</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Storm of Swords</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Feast for Crows</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Dance with Dragons</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>George R. R. Martin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bantam</t>
+    <t>美國國家公園終極探祕 : 公園管理員、當地戶外用品業者與導遊教你如何避開觀光客, 獲得最滿意的體驗</t>
+  </si>
+  <si>
+    <t>國家地理學會叢書部</t>
+  </si>
+  <si>
+    <t>大石國際文化</t>
+  </si>
+  <si>
+    <t>國家地理終極登山裝備指南 : 上山前一定要認識的工具與技巧</t>
+  </si>
+  <si>
+    <t>安德魯.史克卡(Anderw Skurka)</t>
+  </si>
+  <si>
+    <t>全民英檢中級題庫大全</t>
+  </si>
+  <si>
+    <t>馬爾克斯 (Sara K. Marks)</t>
+  </si>
+  <si>
+    <t>英美語言出版</t>
   </si>
 </sst>
 </file>
@@ -114,7 +77,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="183" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -174,7 +137,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -457,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -484,13 +447,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -501,16 +464,16 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <v>1998</v>
+        <v>2013</v>
       </c>
       <c r="F2" s="2">
-        <v>9780439708180</v>
+        <v>9789865918279</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -518,19 +481,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>2000</v>
+        <v>2013</v>
       </c>
       <c r="F3" s="2">
-        <v>9780439064873</v>
+        <v>9789865918187</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -538,199 +501,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>2001</v>
+        <v>2007</v>
       </c>
       <c r="F4" s="2">
-        <v>9780439136365</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>2002</v>
-      </c>
-      <c r="F5" s="2">
-        <v>9780439139601</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>2004</v>
-      </c>
-      <c r="F6" s="2">
-        <v>9780439358071</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7">
-        <v>2006</v>
-      </c>
-      <c r="F7" s="2">
-        <v>9780439785969</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8">
-        <v>2009</v>
-      </c>
-      <c r="F8" s="2">
-        <v>9780545139700</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9">
-        <v>1997</v>
-      </c>
-      <c r="F9" s="2">
-        <v>9780553593716</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10">
-        <v>2000</v>
-      </c>
-      <c r="F10" s="2">
-        <v>9780553579901</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11">
-        <v>2003</v>
-      </c>
-      <c r="F11" s="2">
-        <v>9780553573428</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12">
-        <v>2006</v>
-      </c>
-      <c r="F12" s="2">
-        <v>9780553582024</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13">
-        <v>2013</v>
-      </c>
-      <c r="F13" s="2">
-        <v>9780553582017</v>
+        <v>9789868156982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>